<commit_message>
Añadidos a la documentacion
</commit_message>
<xml_diff>
--- a/ExtraClase/EMNA-Documentacion.xlsx
+++ b/ExtraClase/EMNA-Documentacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sergio_arias8941_uco_net_co/Documents/Desktop/Universidad/uco-2024-2/IS2/IS2/ExtraClase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arias Ramirez\OneDrive\Escritorio\U\2024-2\IS2\ExtraClase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{904820FA-D277-4977-A49B-5EF6DEF442BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7184B4AC-C76D-4CDA-A37E-26AF24B34EBF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307CB99E-3F2C-46F7-99CD-84845706B2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla de Contenido" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="898">
   <si>
     <t>Trade off de QA</t>
   </si>
@@ -3700,6 +3700,66 @@
   <si>
     <t>Descripción paquete</t>
   </si>
+  <si>
+    <t xml:space="preserve">emna </t>
+  </si>
+  <si>
+    <t>emnaMensajesMS</t>
+  </si>
+  <si>
+    <t>emnaUsuariosMS</t>
+  </si>
+  <si>
+    <t>emnaSeguridadMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adaptado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desarrollo </t>
+  </si>
+  <si>
+    <t>Python3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Django </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sqlite </t>
+  </si>
+  <si>
+    <t>Sqlite</t>
+  </si>
+  <si>
+    <t>emna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emna-extraclase </t>
+  </si>
+  <si>
+    <t>emna-extraclase/emna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configuraciones </t>
+  </si>
+  <si>
+    <t xml:space="preserve">migrations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">urls </t>
+  </si>
+  <si>
+    <t xml:space="preserve">views </t>
+  </si>
+  <si>
+    <t xml:space="preserve">models </t>
+  </si>
+  <si>
+    <t xml:space="preserve">serializers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">frontend </t>
+  </si>
 </sst>
 </file>
 
@@ -3954,7 +4014,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -4256,6 +4316,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4264,7 +4342,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -4515,8 +4593,62 @@
     <xf numFmtId="0" fontId="12" fillId="22" borderId="22" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4538,24 +4670,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4623,44 +4737,86 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -7221,7 +7377,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-MX"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7700,7 +7856,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="361250320"/>
@@ -7759,7 +7915,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="361256080"/>
@@ -7801,7 +7957,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-MX"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7838,7 +7994,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-MX"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8435,10 +8591,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{20B912FF-7A15-4BCD-8F27-A1F642484F2B}" name="Tabla12" displayName="Tabla12" ref="A3:J17" totalsRowShown="0" headerRowDxfId="180" dataDxfId="179">
   <autoFilter ref="A3:J17" xr:uid="{20B912FF-7A15-4BCD-8F27-A1F642484F2B}"/>
@@ -8946,8 +9098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8960,72 +9112,72 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
-      <c r="B1" s="136" t="s">
+      <c r="B1" s="101" t="s">
         <v>374</v>
       </c>
-      <c r="C1" s="136"/>
+      <c r="C1" s="101"/>
       <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>375</v>
       </c>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="100" t="s">
         <v>367</v>
       </c>
-      <c r="C2" s="137"/>
+      <c r="C2" s="100"/>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
         <v>376</v>
       </c>
-      <c r="B3" s="137" t="s">
+      <c r="B3" s="100" t="s">
         <v>371</v>
       </c>
-      <c r="C3" s="137"/>
+      <c r="C3" s="100"/>
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>377</v>
       </c>
-      <c r="B4" s="137" t="s">
+      <c r="B4" s="100" t="s">
         <v>383</v>
       </c>
-      <c r="C4" s="137"/>
+      <c r="C4" s="100"/>
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
         <v>368</v>
       </c>
-      <c r="B5" s="137"/>
-      <c r="C5" s="137"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="100"/>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>369</v>
       </c>
-      <c r="B6" s="137" t="s">
+      <c r="B6" s="100" t="s">
         <v>370</v>
       </c>
-      <c r="C6" s="137"/>
+      <c r="C6" s="100"/>
     </row>
     <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
         <v>372</v>
       </c>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="100" t="s">
         <v>373</v>
       </c>
-      <c r="C7" s="137"/>
+      <c r="C7" s="100"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="138" t="s">
+      <c r="A10" s="97" t="s">
         <v>432</v>
       </c>
       <c r="B10" s="18" t="s">
@@ -9057,13 +9209,13 @@
       <c r="A14" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="B14" s="139"/>
+      <c r="B14" s="98"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="140" t="s">
+      <c r="B15" s="99" t="s">
         <v>865</v>
       </c>
     </row>
@@ -9071,7 +9223,7 @@
       <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="140" t="s">
+      <c r="B16" s="99" t="s">
         <v>866</v>
       </c>
     </row>
@@ -11208,74 +11360,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="120" t="s">
         <v>417</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="119" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="119" t="s">
         <v>348</v>
       </c>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -11409,75 +11561,75 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="113"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="125"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="126" t="s">
         <v>314</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="116"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="123" t="s">
         <v>349</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="112"/>
-      <c r="I4" s="113"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="125"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="123" t="s">
         <v>350</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="113"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="124"/>
+      <c r="I5" s="125"/>
       <c r="Q5" s="32"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="121" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="110"/>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
@@ -11642,74 +11794,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="123" t="s">
         <v>428</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="113"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="125"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="126" t="s">
         <v>411</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="116"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="119" t="s">
         <v>343</v>
       </c>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="119" t="s">
         <v>344</v>
       </c>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -11875,74 +12027,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="123" t="s">
         <v>428</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="113"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="125"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="126" t="s">
         <v>412</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="116"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="119" t="s">
         <v>345</v>
       </c>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="119" t="s">
         <v>346</v>
       </c>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -12108,74 +12260,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="123" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="113"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="125"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="126" t="s">
         <v>259</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="116"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="119" t="s">
         <v>339</v>
       </c>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="119" t="s">
         <v>340</v>
       </c>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -12338,74 +12490,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="113"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="125"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="126" t="s">
         <v>260</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="116"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="119" t="s">
         <v>341</v>
       </c>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="119" t="s">
         <v>342</v>
       </c>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -12568,74 +12720,74 @@
       <c r="A2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="119"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="131"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="133" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="132" t="s">
         <v>335</v>
       </c>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
+      <c r="H4" s="132"/>
+      <c r="I4" s="132"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="129" t="s">
         <v>336</v>
       </c>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="119"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="131"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -12775,19 +12927,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517C7F59-370C-4644-9448-B170013D8C24}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:G8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="44" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12797,210 +12946,596 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="94" t="s">
         <v>867</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="94" t="s">
         <v>868</v>
       </c>
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="131"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="130" t="s">
+      <c r="A4" s="94" t="s">
         <v>869</v>
       </c>
-      <c r="B4" s="131"/>
-      <c r="C4" s="131"/>
-      <c r="D4" s="131"/>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="130" t="s">
+      <c r="A5" s="94" t="s">
         <v>870</v>
       </c>
-      <c r="B5" s="131"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="92" t="s">
         <v>874</v>
       </c>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="92" t="s">
         <v>875</v>
       </c>
-      <c r="C6" s="128" t="s">
+      <c r="C6" s="92" t="s">
         <v>876</v>
       </c>
-      <c r="D6" s="128" t="s">
+      <c r="D6" s="92" t="s">
         <v>871</v>
       </c>
-      <c r="E6" s="128" t="s">
+      <c r="E6" s="92" t="s">
         <v>872</v>
       </c>
-      <c r="F6" s="128" t="s">
+      <c r="F6" s="92" t="s">
         <v>877</v>
       </c>
-      <c r="G6" s="128"/>
+      <c r="G6" s="92"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="129"/>
-      <c r="B7" s="129"/>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="131"/>
-      <c r="G7" s="131"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="93" t="s">
+        <v>889</v>
+      </c>
+      <c r="C7" s="93"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="129"/>
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="129"/>
-      <c r="E8" s="129"/>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
+      <c r="A8" s="143" t="str">
+        <f>$B$7</f>
+        <v xml:space="preserve">emna-extraclase </v>
+      </c>
+      <c r="B8" s="93" t="s">
+        <v>878</v>
+      </c>
+      <c r="C8" s="93" t="s">
+        <v>890</v>
+      </c>
+      <c r="D8" s="93" t="str">
+        <f>C11</f>
+        <v>emna-extraclase /emnaMensajesMS</v>
+      </c>
+      <c r="E8" s="93"/>
+      <c r="F8" s="102" t="s">
+        <v>891</v>
+      </c>
+      <c r="G8" s="102"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="129"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="129"/>
-      <c r="E9" s="129"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="131"/>
+      <c r="A9" s="144"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93" t="str">
+        <f>C19</f>
+        <v>emna-extraclase /emnaUsuariosMS</v>
+      </c>
+      <c r="E9" s="93"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="95"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="129"/>
-      <c r="B10" s="129"/>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="129"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="131"/>
+      <c r="A10" s="145"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93" t="str">
+        <f>C27</f>
+        <v>emna-extraclase /emnaSeguridadMS</v>
+      </c>
+      <c r="E10" s="93"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="129"/>
-      <c r="B11" s="129"/>
-      <c r="C11" s="129"/>
-      <c r="D11" s="129"/>
-      <c r="E11" s="129"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="131"/>
+      <c r="A11" s="2" t="str">
+        <f>$B$7</f>
+        <v xml:space="preserve">emna-extraclase </v>
+      </c>
+      <c r="B11" s="93" t="s">
+        <v>879</v>
+      </c>
+      <c r="C11" s="93" t="str">
+        <f>$B$7 &amp; "/"&amp;B11</f>
+        <v>emna-extraclase /emnaMensajesMS</v>
+      </c>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93" t="str">
+        <f>C8</f>
+        <v>emna-extraclase/emna</v>
+      </c>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="129"/>
-      <c r="B12" s="129"/>
-      <c r="C12" s="129"/>
-      <c r="D12" s="129"/>
-      <c r="E12" s="129"/>
-      <c r="F12" s="132"/>
-      <c r="G12" s="132"/>
+      <c r="A12" s="2" t="str">
+        <f>$A$11&amp;"/"&amp;$B$11</f>
+        <v>emna-extraclase /emnaMensajesMS</v>
+      </c>
+      <c r="B12" s="93" t="s">
+        <v>892</v>
+      </c>
+      <c r="C12" s="93" t="str">
+        <f>$C$11 &amp; "/"&amp;B12</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/migrations </v>
+      </c>
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="129"/>
-      <c r="B13" s="129"/>
-      <c r="C13" s="129"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="132"/>
-      <c r="G13" s="132"/>
+      <c r="A13" s="2" t="str">
+        <f t="shared" ref="A13:A17" si="0">$A$11&amp;"/"&amp;$B$11</f>
+        <v>emna-extraclase /emnaMensajesMS</v>
+      </c>
+      <c r="B13" s="93" t="s">
+        <v>893</v>
+      </c>
+      <c r="C13" s="93" t="str">
+        <f>$C$11 &amp; "/"&amp;B13</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/urls </v>
+      </c>
+      <c r="D13" s="93" t="str">
+        <f>C14</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/views </v>
+      </c>
+      <c r="E13" s="93"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="129"/>
-      <c r="B14" s="129"/>
-      <c r="C14" s="129"/>
-      <c r="D14" s="129"/>
-      <c r="E14" s="129"/>
-      <c r="F14" s="132"/>
-      <c r="G14" s="132"/>
+      <c r="A14" s="143" t="str">
+        <f t="shared" si="0"/>
+        <v>emna-extraclase /emnaMensajesMS</v>
+      </c>
+      <c r="B14" s="93" t="s">
+        <v>894</v>
+      </c>
+      <c r="C14" s="93" t="str">
+        <f>$C$11 &amp; "/"&amp;B14</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/views </v>
+      </c>
+      <c r="D14" s="93" t="str">
+        <f>C16</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/serializers </v>
+      </c>
+      <c r="E14" s="93" t="str">
+        <f>C13</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/urls </v>
+      </c>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="129"/>
-      <c r="B15" s="129"/>
-      <c r="C15" s="129"/>
-      <c r="D15" s="129"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="132"/>
-      <c r="G15" s="132"/>
+      <c r="A15" s="145"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="93" t="str">
+        <f>C17</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/models </v>
+      </c>
+      <c r="E15" s="93"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="129"/>
-      <c r="B16" s="129"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="129"/>
-      <c r="E16" s="129"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="132"/>
+      <c r="A16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>emna-extraclase /emnaMensajesMS</v>
+      </c>
+      <c r="B16" s="93" t="s">
+        <v>896</v>
+      </c>
+      <c r="C16" s="93" t="str">
+        <f>$C$11 &amp; "/"&amp;B16</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/serializers </v>
+      </c>
+      <c r="D16" s="93" t="str">
+        <f>C17</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/models </v>
+      </c>
+      <c r="E16" s="93" t="str">
+        <f>C14</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/views </v>
+      </c>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="129"/>
-      <c r="B17" s="129"/>
-      <c r="C17" s="129"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="129"/>
-      <c r="F17" s="132"/>
-      <c r="G17" s="132"/>
+      <c r="A17" s="143" t="str">
+        <f t="shared" si="0"/>
+        <v>emna-extraclase /emnaMensajesMS</v>
+      </c>
+      <c r="B17" s="93" t="s">
+        <v>895</v>
+      </c>
+      <c r="C17" s="93" t="str">
+        <f>$C$11 &amp; "/"&amp;B17</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/models </v>
+      </c>
+      <c r="D17" s="93"/>
+      <c r="E17" s="93" t="str">
+        <f>C14</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/views </v>
+      </c>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="129"/>
-      <c r="B18" s="129"/>
-      <c r="C18" s="129"/>
-      <c r="D18" s="129"/>
-      <c r="E18" s="129"/>
-      <c r="F18" s="132"/>
-      <c r="G18" s="132"/>
+      <c r="A18" s="145"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93" t="str">
+        <f>C16</f>
+        <v xml:space="preserve">emna-extraclase /emnaMensajesMS/serializers </v>
+      </c>
+      <c r="F18" s="96"/>
+      <c r="G18" s="96"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="129"/>
-      <c r="B19" s="129"/>
-      <c r="C19" s="129"/>
-      <c r="D19" s="129"/>
-      <c r="E19" s="129"/>
-      <c r="F19" s="132"/>
-      <c r="G19" s="132"/>
+      <c r="A19" s="2" t="str">
+        <f>$B$7</f>
+        <v xml:space="preserve">emna-extraclase </v>
+      </c>
+      <c r="B19" s="93" t="s">
+        <v>880</v>
+      </c>
+      <c r="C19" s="93" t="str">
+        <f>$B$7 &amp; "/"&amp;B19</f>
+        <v>emna-extraclase /emnaUsuariosMS</v>
+      </c>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="96"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="129"/>
-      <c r="B20" s="129"/>
-      <c r="C20" s="129"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="129"/>
-      <c r="F20" s="132"/>
-      <c r="G20" s="132"/>
+      <c r="A20" s="2" t="str">
+        <f>$A$19&amp;"/"&amp;$B$19</f>
+        <v>emna-extraclase /emnaUsuariosMS</v>
+      </c>
+      <c r="B20" s="93" t="s">
+        <v>892</v>
+      </c>
+      <c r="C20" s="93" t="str">
+        <f>$C$19 &amp; "/"&amp;B20</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/migrations </v>
+      </c>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93" t="str">
+        <f>C8</f>
+        <v>emna-extraclase/emna</v>
+      </c>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="129"/>
-      <c r="B21" s="129"/>
-      <c r="C21" s="129"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="129"/>
-      <c r="F21" s="132"/>
-      <c r="G21" s="132"/>
+      <c r="A21" s="2" t="str">
+        <f>$A$19&amp;"/"&amp;$B$19</f>
+        <v>emna-extraclase /emnaUsuariosMS</v>
+      </c>
+      <c r="B21" s="93" t="s">
+        <v>893</v>
+      </c>
+      <c r="C21" s="93" t="str">
+        <f>$C$19 &amp; "/"&amp;B21</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/urls </v>
+      </c>
+      <c r="D21" s="93" t="str">
+        <f>C22</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/views </v>
+      </c>
+      <c r="E21" s="93"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="96"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="143" t="str">
+        <f>$A$19&amp;"/"&amp;$B$19</f>
+        <v>emna-extraclase /emnaUsuariosMS</v>
+      </c>
+      <c r="B22" s="93" t="s">
+        <v>894</v>
+      </c>
+      <c r="C22" s="93" t="str">
+        <f>$C$19 &amp; "/"&amp;B22</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/views </v>
+      </c>
+      <c r="D22" s="93" t="str">
+        <f>C24</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/serializers </v>
+      </c>
+      <c r="E22" s="93" t="str">
+        <f>C21</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/urls </v>
+      </c>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="145"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="93"/>
+      <c r="D23" s="93" t="str">
+        <f>C25</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/models </v>
+      </c>
+      <c r="E23" s="93"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="str">
+        <f>$A$19&amp;"/"&amp;$B$19</f>
+        <v>emna-extraclase /emnaUsuariosMS</v>
+      </c>
+      <c r="B24" s="93" t="s">
+        <v>896</v>
+      </c>
+      <c r="C24" s="93" t="str">
+        <f>$C$19 &amp; "/"&amp;B24</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/serializers </v>
+      </c>
+      <c r="D24" s="93" t="str">
+        <f>C25</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/models </v>
+      </c>
+      <c r="E24" s="93" t="str">
+        <f>C22</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/views </v>
+      </c>
+      <c r="F24" s="96"/>
+      <c r="G24" s="96"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="143" t="str">
+        <f>$A$19&amp;"/"&amp;$B$19</f>
+        <v>emna-extraclase /emnaUsuariosMS</v>
+      </c>
+      <c r="B25" s="93" t="s">
+        <v>895</v>
+      </c>
+      <c r="C25" s="93" t="str">
+        <f>$C$19 &amp; "/"&amp;B25</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/models </v>
+      </c>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93" t="str">
+        <f>C22</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/views </v>
+      </c>
+      <c r="F25" s="96"/>
+      <c r="G25" s="96"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="145"/>
+      <c r="B26" s="93"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="93" t="str">
+        <f>C24</f>
+        <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/serializers </v>
+      </c>
+      <c r="F26" s="96"/>
+      <c r="G26" s="96"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="str">
+        <f>$B$7</f>
+        <v xml:space="preserve">emna-extraclase </v>
+      </c>
+      <c r="B27" s="93" t="s">
+        <v>881</v>
+      </c>
+      <c r="C27" s="93" t="str">
+        <f>$B$7 &amp; "/"&amp;B27</f>
+        <v>emna-extraclase /emnaSeguridadMS</v>
+      </c>
+      <c r="D27" s="93"/>
+      <c r="E27" s="93" t="str">
+        <f>C8</f>
+        <v>emna-extraclase/emna</v>
+      </c>
+      <c r="F27" s="96"/>
+      <c r="G27" s="96"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="str">
+        <f>$A$27&amp;"/"&amp;$B$27</f>
+        <v>emna-extraclase /emnaSeguridadMS</v>
+      </c>
+      <c r="B28" s="93" t="s">
+        <v>892</v>
+      </c>
+      <c r="C28" s="93" t="str">
+        <f>$C$27 &amp; "/"&amp;B28</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/migrations </v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="str">
+        <f t="shared" ref="A29:A33" si="1">$A$27&amp;"/"&amp;$B$27</f>
+        <v>emna-extraclase /emnaSeguridadMS</v>
+      </c>
+      <c r="B29" s="93" t="s">
+        <v>893</v>
+      </c>
+      <c r="C29" s="93" t="str">
+        <f>$C$27 &amp; "/"&amp;B29</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/urls </v>
+      </c>
+      <c r="D29" s="93" t="str">
+        <f>C30</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/views </v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="143" t="str">
+        <f t="shared" si="1"/>
+        <v>emna-extraclase /emnaSeguridadMS</v>
+      </c>
+      <c r="B30" s="93" t="s">
+        <v>894</v>
+      </c>
+      <c r="C30" s="93" t="str">
+        <f>$C$27 &amp; "/"&amp;B30</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/views </v>
+      </c>
+      <c r="D30" s="93" t="str">
+        <f>C32</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/serializers </v>
+      </c>
+      <c r="E30" s="93" t="str">
+        <f>C29</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/urls </v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="145"/>
+      <c r="B31" s="93"/>
+      <c r="C31" s="93"/>
+      <c r="D31" s="93" t="str">
+        <f>C33</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/models </v>
+      </c>
+      <c r="E31" s="93"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>emna-extraclase /emnaSeguridadMS</v>
+      </c>
+      <c r="B32" s="93" t="s">
+        <v>896</v>
+      </c>
+      <c r="C32" s="93" t="str">
+        <f>$C$27 &amp; "/"&amp;B32</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/serializers </v>
+      </c>
+      <c r="D32" s="93" t="str">
+        <f>C33</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/models </v>
+      </c>
+      <c r="E32" s="93" t="str">
+        <f>C30</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/views </v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="143" t="str">
+        <f t="shared" si="1"/>
+        <v>emna-extraclase /emnaSeguridadMS</v>
+      </c>
+      <c r="B33" s="93" t="s">
+        <v>895</v>
+      </c>
+      <c r="C33" s="93" t="str">
+        <f>$C$27 &amp; "/"&amp;B33</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/models </v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="93" t="str">
+        <f>C30</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/views </v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="145"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="93" t="str">
+        <f>C32</f>
+        <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/serializers </v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="str">
+        <f>$B$7</f>
+        <v xml:space="preserve">emna-extraclase </v>
+      </c>
+      <c r="B35" s="93" t="s">
+        <v>897</v>
+      </c>
+      <c r="C35" s="2" t="str">
+        <f>$B$7 &amp; "/"&amp;B11</f>
+        <v>emna-extraclase /emnaMensajesMS</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
+  <mergeCells count="16">
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
@@ -13012,6 +13547,7 @@
     <hyperlink ref="A1" location="'Tabla de Contenido'!A1" display="Tabla de Contenido" xr:uid="{94EFA083-0C5B-412C-8DD7-22C9E2BEB40A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13037,68 +13573,68 @@
       <c r="A2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="119"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="131"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
+      <c r="B3" s="133"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
+      <c r="B4" s="132"/>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
+      <c r="H4" s="132"/>
+      <c r="I4" s="132"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="117"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="119"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="131"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -13219,74 +13755,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="123" t="s">
         <v>539</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="113"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="125"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="126" t="s">
         <v>271</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="116"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="119" t="s">
         <v>337</v>
       </c>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="119" t="s">
         <v>338</v>
       </c>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -13457,74 +13993,74 @@
       <c r="A2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="134" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="117" t="s">
+      <c r="B3" s="129" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="119"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="131"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="129" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="118"/>
-      <c r="I4" s="119"/>
+      <c r="C4" s="130"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="131"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="132" t="s">
         <v>196</v>
       </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="132"/>
+      <c r="G5" s="132"/>
+      <c r="H5" s="132"/>
+      <c r="I5" s="132"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -13743,74 +14279,74 @@
       <c r="A2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="123" t="s">
         <v>379</v>
       </c>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="125"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="137"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="138" t="s">
         <v>197</v>
       </c>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="125"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="137"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="119" t="s">
         <v>378</v>
       </c>
-      <c r="C5" s="127"/>
-      <c r="D5" s="127"/>
-      <c r="E5" s="127"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="139"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -14674,167 +15210,392 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B1D57B-A645-40E4-A8D4-77A621BBB19C}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="24.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="150" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="150" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="150" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="150" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="24.7109375" style="150"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="146" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="130" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="151" t="s">
         <v>867</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="130" t="s">
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="151" t="s">
         <v>868</v>
       </c>
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="131"/>
-      <c r="F3" s="131"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="130" t="s">
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="151" t="s">
         <v>869</v>
       </c>
-      <c r="B4" s="131"/>
-      <c r="C4" s="131"/>
-      <c r="D4" s="131"/>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="130" t="s">
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="151" t="s">
         <v>870</v>
       </c>
-      <c r="B5" s="131"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="151" t="s">
         <v>465</v>
       </c>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="151" t="s">
         <v>361</v>
       </c>
-      <c r="C6" s="128" t="s">
+      <c r="C6" s="151" t="s">
         <v>871</v>
       </c>
-      <c r="D6" s="128" t="s">
+      <c r="D6" s="151" t="s">
         <v>872</v>
       </c>
-      <c r="E6" s="133" t="s">
+      <c r="E6" s="152" t="s">
         <v>873</v>
       </c>
-      <c r="F6" s="133"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="134"/>
-      <c r="B7" s="135"/>
-      <c r="C7" s="129"/>
-      <c r="D7" s="135"/>
-      <c r="E7" s="131"/>
-      <c r="F7" s="131"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="134"/>
-      <c r="B8" s="135"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="135"/>
-      <c r="E8" s="131"/>
-      <c r="F8" s="131"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="134"/>
-      <c r="B9" s="135"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="135"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="131"/>
-      <c r="B10" s="134"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="131"/>
-      <c r="F10" s="131"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="131"/>
-      <c r="B11" s="134"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="129"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="131"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="131"/>
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="129"/>
-      <c r="E12" s="131"/>
-      <c r="F12" s="131"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="129"/>
-      <c r="B13" s="129"/>
-      <c r="C13" s="129"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="131"/>
-      <c r="F13" s="131"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="129"/>
-      <c r="B14" s="129"/>
-      <c r="C14" s="129"/>
-      <c r="D14" s="129"/>
-      <c r="E14" s="131"/>
-      <c r="F14" s="131"/>
+      <c r="F6" s="152"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="103" t="s">
+        <v>878</v>
+      </c>
+      <c r="B7" s="103" t="s">
+        <v>883</v>
+      </c>
+      <c r="C7" s="96" t="s">
+        <v>884</v>
+      </c>
+      <c r="D7" s="103"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="103"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="96" t="s">
+        <v>885</v>
+      </c>
+      <c r="D8" s="103"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="103"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="96" t="s">
+        <v>887</v>
+      </c>
+      <c r="D9" s="103"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="102" t="s">
+        <v>884</v>
+      </c>
+      <c r="B10" s="103" t="s">
+        <v>882</v>
+      </c>
+      <c r="C10" s="103"/>
+      <c r="D10" s="96" t="s">
+        <v>888</v>
+      </c>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="H10" s="166"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="102"/>
+      <c r="B11" s="103"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="96" t="s">
+        <v>885</v>
+      </c>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="102"/>
+      <c r="B12" s="103"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="96" t="s">
+        <v>887</v>
+      </c>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="103" t="s">
+        <v>885</v>
+      </c>
+      <c r="B13" s="103" t="s">
+        <v>882</v>
+      </c>
+      <c r="C13" s="140" t="s">
+        <v>884</v>
+      </c>
+      <c r="D13" s="96" t="s">
+        <v>888</v>
+      </c>
+      <c r="E13" s="154"/>
+      <c r="F13" s="155"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="103"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="141"/>
+      <c r="D14" s="64" t="s">
+        <v>879</v>
+      </c>
+      <c r="E14" s="156"/>
+      <c r="F14" s="157"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="103"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="141"/>
+      <c r="D15" s="64" t="s">
+        <v>880</v>
+      </c>
+      <c r="E15" s="156"/>
+      <c r="F15" s="157"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="103"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="142"/>
+      <c r="D16" s="64" t="s">
+        <v>881</v>
+      </c>
+      <c r="E16" s="158"/>
+      <c r="F16" s="159"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="103" t="s">
+        <v>886</v>
+      </c>
+      <c r="B17" s="103" t="s">
+        <v>882</v>
+      </c>
+      <c r="C17" s="140" t="s">
+        <v>884</v>
+      </c>
+      <c r="D17" s="96" t="s">
+        <v>888</v>
+      </c>
+      <c r="E17" s="160"/>
+      <c r="F17" s="161"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="103"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="64" t="s">
+        <v>879</v>
+      </c>
+      <c r="E18" s="162"/>
+      <c r="F18" s="163"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="103"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="141"/>
+      <c r="D19" s="64" t="s">
+        <v>880</v>
+      </c>
+      <c r="E19" s="162"/>
+      <c r="F19" s="163"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="103"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="142"/>
+      <c r="D20" s="64" t="s">
+        <v>881</v>
+      </c>
+      <c r="E20" s="164"/>
+      <c r="F20" s="165"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="107" t="s">
+        <v>879</v>
+      </c>
+      <c r="B21" s="107" t="s">
+        <v>883</v>
+      </c>
+      <c r="C21" s="96" t="s">
+        <v>884</v>
+      </c>
+      <c r="D21" s="147" t="s">
+        <v>888</v>
+      </c>
+      <c r="E21" s="160"/>
+      <c r="F21" s="161"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="153"/>
+      <c r="B22" s="153"/>
+      <c r="C22" s="96" t="s">
+        <v>885</v>
+      </c>
+      <c r="D22" s="148"/>
+      <c r="E22" s="162"/>
+      <c r="F22" s="163"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="108"/>
+      <c r="B23" s="108"/>
+      <c r="C23" s="96" t="s">
+        <v>887</v>
+      </c>
+      <c r="D23" s="149"/>
+      <c r="E23" s="164"/>
+      <c r="F23" s="165"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="107" t="s">
+        <v>880</v>
+      </c>
+      <c r="B24" s="107" t="s">
+        <v>883</v>
+      </c>
+      <c r="C24" s="96" t="s">
+        <v>884</v>
+      </c>
+      <c r="D24" s="147" t="s">
+        <v>888</v>
+      </c>
+      <c r="E24" s="160"/>
+      <c r="F24" s="161"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="153"/>
+      <c r="B25" s="153"/>
+      <c r="C25" s="96" t="s">
+        <v>885</v>
+      </c>
+      <c r="D25" s="148"/>
+      <c r="E25" s="162"/>
+      <c r="F25" s="163"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="108"/>
+      <c r="B26" s="108"/>
+      <c r="C26" s="96" t="s">
+        <v>887</v>
+      </c>
+      <c r="D26" s="149"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="165"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="107" t="s">
+        <v>881</v>
+      </c>
+      <c r="B27" s="107" t="s">
+        <v>883</v>
+      </c>
+      <c r="C27" s="96" t="s">
+        <v>884</v>
+      </c>
+      <c r="D27" s="147" t="s">
+        <v>888</v>
+      </c>
+      <c r="E27" s="160"/>
+      <c r="F27" s="161"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="153"/>
+      <c r="B28" s="153"/>
+      <c r="C28" s="96" t="s">
+        <v>885</v>
+      </c>
+      <c r="D28" s="148"/>
+      <c r="E28" s="162"/>
+      <c r="F28" s="163"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="108"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="96" t="s">
+        <v>887</v>
+      </c>
+      <c r="D29" s="149"/>
+      <c r="E29" s="164"/>
+      <c r="F29" s="165"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="E10:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
+  <mergeCells count="33">
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E13:F16"/>
+    <mergeCell ref="E17:F20"/>
+    <mergeCell ref="E21:F23"/>
+    <mergeCell ref="E24:F26"/>
+    <mergeCell ref="E27:F29"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:F9"/>
+    <mergeCell ref="A13:A16"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:F9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="E10:F12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Tabla de Contenido'!A1" display="Tabla de Contenido" xr:uid="{32414F91-C2A5-47DD-93EA-9C2CBC6A25AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15769,914 +16530,914 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="92">
+      <c r="A3" s="104">
         <v>1</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="104" t="s">
         <v>476</v>
       </c>
       <c r="C3" s="75" t="s">
         <v>477</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="92"/>
-      <c r="B4" s="92"/>
+      <c r="A4" s="104"/>
+      <c r="B4" s="104"/>
       <c r="C4" s="75" t="s">
         <v>478</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="92">
+      <c r="A5" s="104">
         <v>2</v>
       </c>
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="104" t="s">
         <v>481</v>
       </c>
       <c r="C5" s="75" t="s">
         <v>482</v>
       </c>
-      <c r="D5" s="92" t="s">
+      <c r="D5" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="92"/>
-      <c r="B6" s="92"/>
+      <c r="A6" s="104"/>
+      <c r="B6" s="104"/>
       <c r="C6" s="75" t="s">
         <v>483</v>
       </c>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="92">
+      <c r="A7" s="104">
         <v>3</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="104" t="s">
         <v>537</v>
       </c>
       <c r="C7" s="75" t="s">
         <v>484</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E7" s="92" t="s">
+      <c r="E7" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="92"/>
-      <c r="B8" s="92"/>
+      <c r="A8" s="104"/>
+      <c r="B8" s="104"/>
       <c r="C8" s="75" t="s">
         <v>485</v>
       </c>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
     </row>
     <row r="9" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="92">
+      <c r="A9" s="104">
         <v>4</v>
       </c>
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="104" t="s">
         <v>486</v>
       </c>
       <c r="C9" s="75" t="s">
         <v>487</v>
       </c>
-      <c r="D9" s="92" t="s">
+      <c r="D9" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="E9" s="92" t="s">
+      <c r="E9" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="92"/>
-      <c r="B10" s="92"/>
+      <c r="A10" s="104"/>
+      <c r="B10" s="104"/>
       <c r="C10" s="75" t="s">
         <v>488</v>
       </c>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
     </row>
     <row r="11" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="92">
+      <c r="A11" s="104">
         <v>5</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="104" t="s">
         <v>543</v>
       </c>
       <c r="C11" s="75" t="s">
         <v>490</v>
       </c>
-      <c r="D11" s="92" t="s">
+      <c r="D11" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E11" s="92" t="s">
+      <c r="E11" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="92"/>
-      <c r="B12" s="92"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="75" t="s">
         <v>491</v>
       </c>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
+      <c r="D12" s="104"/>
+      <c r="E12" s="104"/>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="92">
+      <c r="A13" s="104">
         <v>6</v>
       </c>
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="104" t="s">
         <v>492</v>
       </c>
       <c r="C13" s="75" t="s">
         <v>493</v>
       </c>
-      <c r="D13" s="92" t="s">
+      <c r="D13" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E13" s="92" t="s">
+      <c r="E13" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="92"/>
-      <c r="B14" s="92"/>
+      <c r="A14" s="104"/>
+      <c r="B14" s="104"/>
       <c r="C14" s="75" t="s">
         <v>494</v>
       </c>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
     </row>
     <row r="15" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="92">
+      <c r="A15" s="104">
         <v>7</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="104" t="s">
         <v>495</v>
       </c>
       <c r="C15" s="75" t="s">
         <v>496</v>
       </c>
-      <c r="D15" s="92" t="s">
+      <c r="D15" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E15" s="92" t="s">
+      <c r="E15" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="92"/>
-      <c r="B16" s="92"/>
+      <c r="A16" s="104"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="75" t="s">
         <v>497</v>
       </c>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
     </row>
     <row r="17" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="92">
+      <c r="A17" s="104">
         <v>8</v>
       </c>
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="104" t="s">
         <v>498</v>
       </c>
       <c r="C17" s="75" t="s">
         <v>499</v>
       </c>
-      <c r="D17" s="92" t="s">
+      <c r="D17" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E17" s="92" t="s">
+      <c r="E17" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
-      <c r="B18" s="92"/>
+      <c r="A18" s="104"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="75" t="s">
         <v>500</v>
       </c>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="92">
+      <c r="A19" s="104">
         <v>9</v>
       </c>
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="104" t="s">
         <v>501</v>
       </c>
       <c r="C19" s="75" t="s">
         <v>502</v>
       </c>
-      <c r="D19" s="92" t="s">
+      <c r="D19" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E19" s="92" t="s">
+      <c r="E19" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="92"/>
-      <c r="B20" s="92"/>
+      <c r="A20" s="104"/>
+      <c r="B20" s="104"/>
       <c r="C20" s="75" t="s">
         <v>503</v>
       </c>
-      <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
     </row>
     <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="92">
+      <c r="A21" s="104">
         <v>10</v>
       </c>
-      <c r="B21" s="92" t="s">
+      <c r="B21" s="104" t="s">
         <v>504</v>
       </c>
       <c r="C21" s="75" t="s">
         <v>505</v>
       </c>
-      <c r="D21" s="92" t="s">
+      <c r="D21" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="E21" s="92" t="s">
+      <c r="E21" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="92"/>
-      <c r="B22" s="92"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="75" t="s">
         <v>506</v>
       </c>
-      <c r="D22" s="92"/>
-      <c r="E22" s="92"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="92">
+      <c r="A23" s="104">
         <v>11</v>
       </c>
-      <c r="B23" s="92" t="s">
+      <c r="B23" s="104" t="s">
         <v>507</v>
       </c>
       <c r="C23" s="75" t="s">
         <v>508</v>
       </c>
-      <c r="D23" s="92" t="s">
+      <c r="D23" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E23" s="92" t="s">
+      <c r="E23" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
-      <c r="B24" s="92"/>
+      <c r="A24" s="104"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="75" t="s">
         <v>509</v>
       </c>
-      <c r="D24" s="92"/>
-      <c r="E24" s="92"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="92">
+      <c r="A25" s="104">
         <v>12</v>
       </c>
-      <c r="B25" s="92" t="s">
+      <c r="B25" s="104" t="s">
         <v>510</v>
       </c>
       <c r="C25" s="75" t="s">
         <v>511</v>
       </c>
-      <c r="D25" s="92" t="s">
+      <c r="D25" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="E25" s="92" t="s">
+      <c r="E25" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="92"/>
-      <c r="B26" s="92"/>
+      <c r="A26" s="104"/>
+      <c r="B26" s="104"/>
       <c r="C26" s="75" t="s">
         <v>512</v>
       </c>
-      <c r="D26" s="92"/>
-      <c r="E26" s="92"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="104"/>
     </row>
     <row r="27" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="92">
+      <c r="A27" s="104">
         <v>13</v>
       </c>
-      <c r="B27" s="92" t="s">
+      <c r="B27" s="104" t="s">
         <v>513</v>
       </c>
       <c r="C27" s="75" t="s">
         <v>514</v>
       </c>
-      <c r="D27" s="92" t="s">
+      <c r="D27" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E27" s="92" t="s">
+      <c r="E27" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="92"/>
-      <c r="B28" s="92"/>
+      <c r="A28" s="104"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="75" t="s">
         <v>515</v>
       </c>
-      <c r="D28" s="92"/>
-      <c r="E28" s="92"/>
+      <c r="D28" s="104"/>
+      <c r="E28" s="104"/>
     </row>
     <row r="29" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="92">
+      <c r="A29" s="104">
         <v>14</v>
       </c>
-      <c r="B29" s="92" t="s">
+      <c r="B29" s="104" t="s">
         <v>516</v>
       </c>
       <c r="C29" s="75" t="s">
         <v>517</v>
       </c>
-      <c r="D29" s="92" t="s">
+      <c r="D29" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="E29" s="92" t="s">
+      <c r="E29" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="92"/>
-      <c r="B30" s="92"/>
+      <c r="A30" s="104"/>
+      <c r="B30" s="104"/>
       <c r="C30" s="75" t="s">
         <v>518</v>
       </c>
-      <c r="D30" s="92"/>
-      <c r="E30" s="92"/>
+      <c r="D30" s="104"/>
+      <c r="E30" s="104"/>
     </row>
     <row r="31" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="92">
+      <c r="A31" s="104">
         <v>15</v>
       </c>
-      <c r="B31" s="92" t="s">
+      <c r="B31" s="104" t="s">
         <v>519</v>
       </c>
       <c r="C31" s="75" t="s">
         <v>520</v>
       </c>
-      <c r="D31" s="92" t="s">
+      <c r="D31" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E31" s="92" t="s">
+      <c r="E31" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="92"/>
-      <c r="B32" s="92"/>
+      <c r="A32" s="104"/>
+      <c r="B32" s="104"/>
       <c r="C32" s="75" t="s">
         <v>521</v>
       </c>
-      <c r="D32" s="92"/>
-      <c r="E32" s="92"/>
+      <c r="D32" s="104"/>
+      <c r="E32" s="104"/>
     </row>
     <row r="33" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="92">
+      <c r="A33" s="104">
         <v>16</v>
       </c>
-      <c r="B33" s="92" t="s">
+      <c r="B33" s="104" t="s">
         <v>522</v>
       </c>
       <c r="C33" s="75" t="s">
         <v>523</v>
       </c>
-      <c r="D33" s="92" t="s">
+      <c r="D33" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E33" s="92" t="s">
+      <c r="E33" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="92"/>
-      <c r="B34" s="92"/>
+      <c r="A34" s="104"/>
+      <c r="B34" s="104"/>
       <c r="C34" s="75" t="s">
         <v>524</v>
       </c>
-      <c r="D34" s="92"/>
-      <c r="E34" s="92"/>
+      <c r="D34" s="104"/>
+      <c r="E34" s="104"/>
     </row>
     <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="92">
+      <c r="A35" s="104">
         <v>17</v>
       </c>
-      <c r="B35" s="92" t="s">
+      <c r="B35" s="104" t="s">
         <v>525</v>
       </c>
       <c r="C35" s="75" t="s">
         <v>526</v>
       </c>
-      <c r="D35" s="92" t="s">
+      <c r="D35" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E35" s="92" t="s">
+      <c r="E35" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="92"/>
-      <c r="B36" s="92"/>
+      <c r="A36" s="104"/>
+      <c r="B36" s="104"/>
       <c r="C36" s="75" t="s">
         <v>527</v>
       </c>
-      <c r="D36" s="92"/>
-      <c r="E36" s="92"/>
+      <c r="D36" s="104"/>
+      <c r="E36" s="104"/>
     </row>
     <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="92">
+      <c r="A37" s="104">
         <v>18</v>
       </c>
-      <c r="B37" s="92" t="s">
+      <c r="B37" s="104" t="s">
         <v>528</v>
       </c>
       <c r="C37" s="75" t="s">
         <v>529</v>
       </c>
-      <c r="D37" s="92" t="s">
+      <c r="D37" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="E37" s="92" t="s">
+      <c r="E37" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="92"/>
-      <c r="B38" s="92"/>
+      <c r="A38" s="104"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="75" t="s">
         <v>530</v>
       </c>
-      <c r="D38" s="92"/>
-      <c r="E38" s="92"/>
+      <c r="D38" s="104"/>
+      <c r="E38" s="104"/>
     </row>
     <row r="39" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="92">
+      <c r="A39" s="104">
         <v>19</v>
       </c>
-      <c r="B39" s="92" t="s">
+      <c r="B39" s="104" t="s">
         <v>531</v>
       </c>
       <c r="C39" s="75" t="s">
         <v>532</v>
       </c>
-      <c r="D39" s="92" t="s">
+      <c r="D39" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E39" s="92" t="s">
+      <c r="E39" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="92"/>
-      <c r="B40" s="92"/>
+      <c r="A40" s="104"/>
+      <c r="B40" s="104"/>
       <c r="C40" s="75" t="s">
         <v>533</v>
       </c>
-      <c r="D40" s="92"/>
-      <c r="E40" s="92"/>
+      <c r="D40" s="104"/>
+      <c r="E40" s="104"/>
     </row>
     <row r="41" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="92">
+      <c r="A41" s="104">
         <v>20</v>
       </c>
-      <c r="B41" s="92" t="s">
+      <c r="B41" s="104" t="s">
         <v>534</v>
       </c>
       <c r="C41" s="75" t="s">
         <v>535</v>
       </c>
-      <c r="D41" s="92" t="s">
+      <c r="D41" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E41" s="92" t="s">
+      <c r="E41" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="92"/>
-      <c r="B42" s="92"/>
+      <c r="A42" s="104"/>
+      <c r="B42" s="104"/>
       <c r="C42" s="75" t="s">
         <v>536</v>
       </c>
-      <c r="D42" s="92"/>
-      <c r="E42" s="92"/>
+      <c r="D42" s="104"/>
+      <c r="E42" s="104"/>
     </row>
     <row r="43" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="92">
+      <c r="A43" s="104">
         <v>21</v>
       </c>
-      <c r="B43" s="92" t="s">
+      <c r="B43" s="104" t="s">
         <v>551</v>
       </c>
       <c r="C43" s="75" t="s">
         <v>552</v>
       </c>
-      <c r="D43" s="92" t="s">
+      <c r="D43" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="E43" s="92" t="s">
+      <c r="E43" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="92"/>
-      <c r="B44" s="92"/>
+      <c r="A44" s="104"/>
+      <c r="B44" s="104"/>
       <c r="C44" s="75" t="s">
         <v>553</v>
       </c>
-      <c r="D44" s="92"/>
-      <c r="E44" s="92"/>
+      <c r="D44" s="104"/>
+      <c r="E44" s="104"/>
     </row>
     <row r="45" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="92">
+      <c r="A45" s="104">
         <v>22</v>
       </c>
-      <c r="B45" s="92" t="s">
+      <c r="B45" s="104" t="s">
         <v>554</v>
       </c>
       <c r="C45" s="75" t="s">
         <v>555</v>
       </c>
-      <c r="D45" s="92" t="s">
+      <c r="D45" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="E45" s="92" t="s">
+      <c r="E45" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="92"/>
-      <c r="B46" s="92"/>
+      <c r="A46" s="104"/>
+      <c r="B46" s="104"/>
       <c r="C46" s="75" t="s">
         <v>556</v>
       </c>
-      <c r="D46" s="92"/>
-      <c r="E46" s="92"/>
+      <c r="D46" s="104"/>
+      <c r="E46" s="104"/>
     </row>
     <row r="47" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="92">
+      <c r="A47" s="104">
         <v>23</v>
       </c>
-      <c r="B47" s="92" t="s">
+      <c r="B47" s="104" t="s">
         <v>557</v>
       </c>
       <c r="C47" s="75" t="s">
         <v>558</v>
       </c>
-      <c r="D47" s="92" t="s">
+      <c r="D47" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E47" s="92" t="s">
+      <c r="E47" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="92"/>
-      <c r="B48" s="92"/>
+      <c r="A48" s="104"/>
+      <c r="B48" s="104"/>
       <c r="C48" s="75" t="s">
         <v>559</v>
       </c>
-      <c r="D48" s="92"/>
-      <c r="E48" s="92"/>
+      <c r="D48" s="104"/>
+      <c r="E48" s="104"/>
     </row>
     <row r="49" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="92">
+      <c r="A49" s="104">
         <v>24</v>
       </c>
-      <c r="B49" s="92" t="s">
+      <c r="B49" s="104" t="s">
         <v>560</v>
       </c>
       <c r="C49" s="75" t="s">
         <v>561</v>
       </c>
-      <c r="D49" s="92" t="s">
+      <c r="D49" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E49" s="92" t="s">
+      <c r="E49" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="92"/>
-      <c r="B50" s="92"/>
+      <c r="A50" s="104"/>
+      <c r="B50" s="104"/>
       <c r="C50" s="75" t="s">
         <v>562</v>
       </c>
-      <c r="D50" s="92"/>
-      <c r="E50" s="92"/>
+      <c r="D50" s="104"/>
+      <c r="E50" s="104"/>
     </row>
     <row r="51" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="92">
+      <c r="A51" s="104">
         <v>25</v>
       </c>
-      <c r="B51" s="92" t="s">
+      <c r="B51" s="104" t="s">
         <v>563</v>
       </c>
       <c r="C51" s="75" t="s">
         <v>564</v>
       </c>
-      <c r="D51" s="92" t="s">
+      <c r="D51" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E51" s="92" t="s">
+      <c r="E51" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="92"/>
-      <c r="B52" s="92"/>
+      <c r="A52" s="104"/>
+      <c r="B52" s="104"/>
       <c r="C52" s="75" t="s">
         <v>565</v>
       </c>
-      <c r="D52" s="92"/>
-      <c r="E52" s="92"/>
+      <c r="D52" s="104"/>
+      <c r="E52" s="104"/>
     </row>
     <row r="53" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="92">
+      <c r="A53" s="104">
         <v>26</v>
       </c>
-      <c r="B53" s="92" t="s">
+      <c r="B53" s="104" t="s">
         <v>566</v>
       </c>
       <c r="C53" s="75" t="s">
         <v>567</v>
       </c>
-      <c r="D53" s="92" t="s">
+      <c r="D53" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E53" s="92" t="s">
+      <c r="E53" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="92"/>
-      <c r="B54" s="92"/>
+      <c r="A54" s="104"/>
+      <c r="B54" s="104"/>
       <c r="C54" s="75" t="s">
         <v>568</v>
       </c>
-      <c r="D54" s="92"/>
-      <c r="E54" s="92"/>
+      <c r="D54" s="104"/>
+      <c r="E54" s="104"/>
     </row>
     <row r="55" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="92">
+      <c r="A55" s="104">
         <v>27</v>
       </c>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="104" t="s">
         <v>569</v>
       </c>
       <c r="C55" s="75" t="s">
         <v>570</v>
       </c>
-      <c r="D55" s="92" t="s">
+      <c r="D55" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="E55" s="92" t="s">
+      <c r="E55" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="92"/>
-      <c r="B56" s="92"/>
+      <c r="A56" s="104"/>
+      <c r="B56" s="104"/>
       <c r="C56" s="75" t="s">
         <v>571</v>
       </c>
-      <c r="D56" s="92"/>
-      <c r="E56" s="92"/>
+      <c r="D56" s="104"/>
+      <c r="E56" s="104"/>
     </row>
     <row r="57" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="92">
+      <c r="A57" s="104">
         <v>28</v>
       </c>
-      <c r="B57" s="92" t="s">
+      <c r="B57" s="104" t="s">
         <v>572</v>
       </c>
       <c r="C57" s="75" t="s">
         <v>573</v>
       </c>
-      <c r="D57" s="92" t="s">
+      <c r="D57" s="104" t="s">
         <v>575</v>
       </c>
-      <c r="E57" s="92" t="s">
+      <c r="E57" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="92"/>
-      <c r="B58" s="92"/>
+      <c r="A58" s="104"/>
+      <c r="B58" s="104"/>
       <c r="C58" s="75" t="s">
         <v>574</v>
       </c>
-      <c r="D58" s="92"/>
-      <c r="E58" s="92"/>
+      <c r="D58" s="104"/>
+      <c r="E58" s="104"/>
     </row>
     <row r="59" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="92">
+      <c r="A59" s="104">
         <v>29</v>
       </c>
-      <c r="B59" s="92" t="s">
+      <c r="B59" s="104" t="s">
         <v>576</v>
       </c>
       <c r="C59" s="75" t="s">
         <v>577</v>
       </c>
-      <c r="D59" s="92" t="s">
+      <c r="D59" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E59" s="92" t="s">
+      <c r="E59" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="92"/>
-      <c r="B60" s="92"/>
+      <c r="A60" s="104"/>
+      <c r="B60" s="104"/>
       <c r="C60" s="75" t="s">
         <v>578</v>
       </c>
-      <c r="D60" s="92"/>
-      <c r="E60" s="92"/>
+      <c r="D60" s="104"/>
+      <c r="E60" s="104"/>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="92">
+      <c r="A61" s="104">
         <v>30</v>
       </c>
-      <c r="B61" s="92" t="s">
+      <c r="B61" s="104" t="s">
         <v>579</v>
       </c>
       <c r="C61" s="75" t="s">
         <v>580</v>
       </c>
-      <c r="D61" s="92" t="s">
+      <c r="D61" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="E61" s="92" t="s">
+      <c r="E61" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="92"/>
-      <c r="B62" s="92"/>
+      <c r="A62" s="104"/>
+      <c r="B62" s="104"/>
       <c r="C62" s="75" t="s">
         <v>581</v>
       </c>
-      <c r="D62" s="92"/>
-      <c r="E62" s="92"/>
+      <c r="D62" s="104"/>
+      <c r="E62" s="104"/>
     </row>
     <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="92">
+      <c r="A63" s="104">
         <v>31</v>
       </c>
-      <c r="B63" s="92" t="s">
+      <c r="B63" s="104" t="s">
         <v>582</v>
       </c>
       <c r="C63" s="75" t="s">
         <v>583</v>
       </c>
-      <c r="D63" s="92" t="s">
+      <c r="D63" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="E63" s="92" t="s">
+      <c r="E63" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="92"/>
-      <c r="B64" s="92"/>
+      <c r="A64" s="104"/>
+      <c r="B64" s="104"/>
       <c r="C64" s="75" t="s">
         <v>584</v>
       </c>
-      <c r="D64" s="92"/>
-      <c r="E64" s="92"/>
+      <c r="D64" s="104"/>
+      <c r="E64" s="104"/>
     </row>
     <row r="65" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="92">
+      <c r="A65" s="104">
         <v>32</v>
       </c>
-      <c r="B65" s="92" t="s">
+      <c r="B65" s="104" t="s">
         <v>585</v>
       </c>
       <c r="C65" s="75" t="s">
         <v>586</v>
       </c>
-      <c r="D65" s="92" t="s">
+      <c r="D65" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="E65" s="92" t="s">
+      <c r="E65" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="92"/>
-      <c r="B66" s="92"/>
+      <c r="A66" s="104"/>
+      <c r="B66" s="104"/>
       <c r="C66" s="75" t="s">
         <v>587</v>
       </c>
-      <c r="D66" s="92"/>
-      <c r="E66" s="92"/>
+      <c r="D66" s="104"/>
+      <c r="E66" s="104"/>
     </row>
     <row r="67" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="92">
+      <c r="A67" s="104">
         <v>33</v>
       </c>
-      <c r="B67" s="92" t="s">
+      <c r="B67" s="104" t="s">
         <v>588</v>
       </c>
       <c r="C67" s="75" t="s">
         <v>589</v>
       </c>
-      <c r="D67" s="92" t="s">
+      <c r="D67" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E67" s="92" t="s">
+      <c r="E67" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="92"/>
-      <c r="B68" s="92"/>
+      <c r="A68" s="104"/>
+      <c r="B68" s="104"/>
       <c r="C68" s="75" t="s">
         <v>590</v>
       </c>
-      <c r="D68" s="92"/>
-      <c r="E68" s="92"/>
+      <c r="D68" s="104"/>
+      <c r="E68" s="104"/>
     </row>
     <row r="69" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="92">
+      <c r="A69" s="104">
         <v>34</v>
       </c>
-      <c r="B69" s="92" t="s">
+      <c r="B69" s="104" t="s">
         <v>591</v>
       </c>
       <c r="C69" s="75" t="s">
         <v>592</v>
       </c>
-      <c r="D69" s="92" t="s">
+      <c r="D69" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E69" s="92" t="s">
+      <c r="E69" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="92"/>
-      <c r="B70" s="92"/>
+      <c r="A70" s="104"/>
+      <c r="B70" s="104"/>
       <c r="C70" s="75" t="s">
         <v>593</v>
       </c>
-      <c r="D70" s="92"/>
-      <c r="E70" s="92"/>
+      <c r="D70" s="104"/>
+      <c r="E70" s="104"/>
     </row>
     <row r="71" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="92">
+      <c r="A71" s="104">
         <v>35</v>
       </c>
-      <c r="B71" s="92" t="s">
+      <c r="B71" s="104" t="s">
         <v>594</v>
       </c>
       <c r="C71" s="75" t="s">
         <v>595</v>
       </c>
-      <c r="D71" s="92" t="s">
+      <c r="D71" s="104" t="s">
         <v>479</v>
       </c>
-      <c r="E71" s="92" t="s">
+      <c r="E71" s="104" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="92"/>
-      <c r="B72" s="92"/>
+      <c r="A72" s="104"/>
+      <c r="B72" s="104"/>
       <c r="C72" s="75" t="s">
         <v>596</v>
       </c>
-      <c r="D72" s="92"/>
-      <c r="E72" s="92"/>
+      <c r="D72" s="104"/>
+      <c r="E72" s="104"/>
     </row>
     <row r="74" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16698,36 +17459,92 @@
     <row r="108" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="140">
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="A23:A24"/>
@@ -16752,92 +17569,36 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Tabla de Contenido'!A1" display="Tabla de Contenido" xr:uid="{39E8F964-FA78-451F-AA99-AC92C3995828}"/>
@@ -16883,54 +17644,54 @@
       <c r="A2" s="29"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="111" t="s">
         <v>437</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="113" t="s">
         <v>438</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="113" t="s">
         <v>439</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="113" t="s">
         <v>440</v>
       </c>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="97"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="115"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="94"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96" t="s">
+      <c r="A4" s="112"/>
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114" t="s">
         <v>441</v>
       </c>
-      <c r="E4" s="96" t="s">
+      <c r="E4" s="114" t="s">
         <v>442</v>
       </c>
-      <c r="F4" s="96" t="s">
+      <c r="F4" s="114" t="s">
         <v>443</v>
       </c>
-      <c r="G4" s="98" t="s">
+      <c r="G4" s="116" t="s">
         <v>444</v>
       </c>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="99"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="117"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="94"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
       <c r="G5" s="62" t="s">
         <v>445</v>
       </c>
@@ -17559,54 +18320,54 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="93" t="s">
+      <c r="A50" s="111" t="s">
         <v>437</v>
       </c>
-      <c r="B50" s="95" t="s">
+      <c r="B50" s="113" t="s">
         <v>438</v>
       </c>
-      <c r="C50" s="95" t="s">
+      <c r="C50" s="113" t="s">
         <v>439</v>
       </c>
-      <c r="D50" s="95" t="s">
+      <c r="D50" s="113" t="s">
         <v>440</v>
       </c>
-      <c r="E50" s="95"/>
-      <c r="F50" s="95"/>
-      <c r="G50" s="95"/>
-      <c r="H50" s="95"/>
-      <c r="I50" s="95"/>
-      <c r="J50" s="95"/>
-      <c r="K50" s="97"/>
+      <c r="E50" s="113"/>
+      <c r="F50" s="113"/>
+      <c r="G50" s="113"/>
+      <c r="H50" s="113"/>
+      <c r="I50" s="113"/>
+      <c r="J50" s="113"/>
+      <c r="K50" s="115"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="94"/>
-      <c r="B51" s="96"/>
-      <c r="C51" s="96"/>
-      <c r="D51" s="96" t="s">
+      <c r="A51" s="112"/>
+      <c r="B51" s="114"/>
+      <c r="C51" s="114"/>
+      <c r="D51" s="114" t="s">
         <v>441</v>
       </c>
-      <c r="E51" s="96" t="s">
+      <c r="E51" s="114" t="s">
         <v>442</v>
       </c>
-      <c r="F51" s="96" t="s">
+      <c r="F51" s="114" t="s">
         <v>443</v>
       </c>
-      <c r="G51" s="98" t="s">
+      <c r="G51" s="116" t="s">
         <v>444</v>
       </c>
-      <c r="H51" s="98"/>
-      <c r="I51" s="98"/>
-      <c r="J51" s="98"/>
-      <c r="K51" s="99"/>
+      <c r="H51" s="116"/>
+      <c r="I51" s="116"/>
+      <c r="J51" s="116"/>
+      <c r="K51" s="117"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="94"/>
-      <c r="B52" s="96"/>
-      <c r="C52" s="96"/>
-      <c r="D52" s="96"/>
-      <c r="E52" s="96"/>
-      <c r="F52" s="96"/>
+      <c r="A52" s="112"/>
+      <c r="B52" s="114"/>
+      <c r="C52" s="114"/>
+      <c r="D52" s="114"/>
+      <c r="E52" s="114"/>
+      <c r="F52" s="114"/>
       <c r="G52" s="62" t="s">
         <v>445</v>
       </c>
@@ -17624,13 +18385,13 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="100" t="s">
+      <c r="A53" s="105" t="s">
         <v>450</v>
       </c>
-      <c r="B53" s="102" t="s">
+      <c r="B53" s="107" t="s">
         <v>451</v>
       </c>
-      <c r="C53" s="104" t="s">
+      <c r="C53" s="109" t="s">
         <v>452</v>
       </c>
       <c r="D53" s="64">
@@ -17659,9 +18420,9 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="101"/>
-      <c r="B54" s="103"/>
-      <c r="C54" s="105"/>
+      <c r="A54" s="106"/>
+      <c r="B54" s="108"/>
+      <c r="C54" s="110"/>
       <c r="D54" s="66">
         <v>2</v>
       </c>
@@ -17916,17 +18677,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="D50:K50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:K51"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
@@ -17935,6 +18685,17 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:K4"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:K51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="C50:C52"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>

</xml_diff>